<commit_message>
ahp data dim1-5 completed + missing analysis
</commit_message>
<xml_diff>
--- a/dataset_generation/missing_analysis/Missings_General.xlsx
+++ b/dataset_generation/missing_analysis/Missings_General.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t xml:space="preserve">variable</t>
   </si>
@@ -248,7 +248,52 @@
     <t xml:space="preserve">ahu_12m_female</t>
   </si>
   <si>
+    <t xml:space="preserve">heq</t>
+  </si>
+  <si>
     <t xml:space="preserve">gini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">median_age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aged65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aged70_male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aged70_female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ext_poverty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">life_expectancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schooling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">literacy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">urban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dependency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homicide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">net_migration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hdi</t>
   </si>
 </sst>
 </file>
@@ -593,7 +638,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.42269142293789</v>
+        <v>0.222582738481506</v>
       </c>
     </row>
     <row r="3">
@@ -609,7 +654,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="5">
@@ -617,7 +662,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="6">
@@ -625,7 +670,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="7">
@@ -633,7 +678,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="8">
@@ -641,7 +686,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="9">
@@ -649,7 +694,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="10">
@@ -657,7 +702,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="11">
@@ -665,7 +710,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="12">
@@ -673,7 +718,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="13">
@@ -681,7 +726,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="14">
@@ -689,7 +734,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="15">
@@ -697,7 +742,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="16">
@@ -705,7 +750,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="17">
@@ -713,7 +758,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="18">
@@ -721,7 +766,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="19">
@@ -729,7 +774,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="20">
@@ -737,7 +782,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="21">
@@ -745,7 +790,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="22">
@@ -753,7 +798,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="23">
@@ -761,7 +806,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="24">
@@ -769,7 +814,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="25">
@@ -777,7 +822,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="26">
@@ -785,7 +830,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="27">
@@ -793,7 +838,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="28">
@@ -801,7 +846,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="29">
@@ -809,7 +854,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="30">
@@ -817,7 +862,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="n">
-        <v>0.317408807098258</v>
+        <v>0.636534717715769</v>
       </c>
     </row>
     <row r="31">
@@ -825,7 +870,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="n">
-        <v>0.559686164968781</v>
+        <v>0.762773091066407</v>
       </c>
     </row>
     <row r="32">
@@ -833,7 +878,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="n">
-        <v>0.560384488991127</v>
+        <v>0.763140817650876</v>
       </c>
     </row>
     <row r="33">
@@ -841,7 +886,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="n">
-        <v>0.602160696680907</v>
+        <v>0.78537746052347</v>
       </c>
     </row>
     <row r="34">
@@ -849,7 +894,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="n">
-        <v>0.641677620768978</v>
+        <v>0.806727233398226</v>
       </c>
     </row>
     <row r="35">
@@ -857,7 +902,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="n">
-        <v>0.581046664475846</v>
+        <v>0.774042829331603</v>
       </c>
     </row>
     <row r="36">
@@ -865,7 +910,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="n">
-        <v>0.759735458429182</v>
+        <v>0.869370538611291</v>
       </c>
     </row>
     <row r="37">
@@ -873,7 +918,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="n">
-        <v>0.937520538941834</v>
+        <v>0.965801427644387</v>
       </c>
     </row>
     <row r="38">
@@ -881,7 +926,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="n">
-        <v>0.937520538941834</v>
+        <v>0.965801427644387</v>
       </c>
     </row>
     <row r="39">
@@ -889,7 +934,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="n">
-        <v>0.937520538941834</v>
+        <v>0.965801427644387</v>
       </c>
     </row>
     <row r="40">
@@ -897,7 +942,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="n">
-        <v>0.577267499178442</v>
+        <v>0.77255029201817</v>
       </c>
     </row>
     <row r="41">
@@ -905,7 +950,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="n">
-        <v>0.577760433782452</v>
+        <v>0.772809863724854</v>
       </c>
     </row>
     <row r="42">
@@ -913,7 +958,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="n">
-        <v>0.577801511666119</v>
+        <v>0.772831494700411</v>
       </c>
     </row>
     <row r="43">
@@ -921,7 +966,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="n">
-        <v>0.577760433782452</v>
+        <v>0.772809863724854</v>
       </c>
     </row>
     <row r="44">
@@ -929,7 +974,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="n">
-        <v>0.68485047650345</v>
+        <v>0.829699329439758</v>
       </c>
     </row>
     <row r="45">
@@ -937,7 +982,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="n">
-        <v>0.577760433782452</v>
+        <v>0.772809863724854</v>
       </c>
     </row>
     <row r="46">
@@ -945,7 +990,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="n">
-        <v>0.952842589549786</v>
+        <v>0.974129353233831</v>
       </c>
     </row>
     <row r="47">
@@ -953,7 +998,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="n">
-        <v>0.990059152152481</v>
+        <v>0.994570625135194</v>
       </c>
     </row>
     <row r="48">
@@ -961,7 +1006,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="n">
-        <v>0.97071146894512</v>
+        <v>0.983928185161151</v>
       </c>
     </row>
     <row r="49">
@@ -969,7 +1014,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="n">
-        <v>0.97071146894512</v>
+        <v>0.983928185161151</v>
       </c>
     </row>
     <row r="50">
@@ -977,7 +1022,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="n">
-        <v>0.97071146894512</v>
+        <v>0.983928185161151</v>
       </c>
     </row>
     <row r="51">
@@ -985,7 +1030,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="n">
-        <v>0.989032205060795</v>
+        <v>0.994029850746269</v>
       </c>
     </row>
     <row r="52">
@@ -993,7 +1038,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="n">
-        <v>0.98878573775879</v>
+        <v>0.993813540990699</v>
       </c>
     </row>
     <row r="53">
@@ -1001,7 +1046,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="n">
-        <v>0.989196516595465</v>
+        <v>0.994116374648497</v>
       </c>
     </row>
     <row r="54">
@@ -1009,7 +1054,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="n">
-        <v>0.992195202103187</v>
+        <v>0.995695435864157</v>
       </c>
     </row>
     <row r="55">
@@ -1017,7 +1062,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="n">
-        <v>0.992195202103187</v>
+        <v>0.995695435864157</v>
       </c>
     </row>
     <row r="56">
@@ -1025,7 +1070,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="n">
-        <v>0.992195202103187</v>
+        <v>0.995695435864157</v>
       </c>
     </row>
     <row r="57">
@@ -1033,7 +1078,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="n">
-        <v>0.987471245481433</v>
+        <v>0.992991563919533</v>
       </c>
     </row>
     <row r="58">
@@ -1041,7 +1086,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="n">
-        <v>0.987882024318107</v>
+        <v>0.993207873675103</v>
       </c>
     </row>
     <row r="59">
@@ -1049,7 +1094,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="n">
-        <v>0.988703581991456</v>
+        <v>0.993640493186243</v>
       </c>
     </row>
     <row r="60">
@@ -1057,7 +1102,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="n">
-        <v>0.985376273414393</v>
+        <v>0.992018170019468</v>
       </c>
     </row>
     <row r="61">
@@ -1065,7 +1110,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="n">
-        <v>0.986937232993756</v>
+        <v>0.992710361237292</v>
       </c>
     </row>
     <row r="62">
@@ -1073,7 +1118,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="n">
-        <v>0.987265856063095</v>
+        <v>0.993099718797318</v>
       </c>
     </row>
     <row r="63">
@@ -1081,7 +1126,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="n">
-        <v>0.988005257969109</v>
+        <v>0.993489076357344</v>
       </c>
     </row>
     <row r="64">
@@ -1089,7 +1134,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="n">
-        <v>0.986855077226421</v>
+        <v>0.992883409041748</v>
       </c>
     </row>
     <row r="65">
@@ -1097,7 +1142,7 @@
         <v>65</v>
       </c>
       <c r="B65" t="n">
-        <v>0.987101544528426</v>
+        <v>0.99301319489509</v>
       </c>
     </row>
     <row r="66">
@@ -1105,7 +1150,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="n">
-        <v>0.976174827472888</v>
+        <v>0.98695652173913</v>
       </c>
     </row>
     <row r="67">
@@ -1113,7 +1158,7 @@
         <v>67</v>
       </c>
       <c r="B67" t="n">
-        <v>0.992195202103187</v>
+        <v>0.995695435864157</v>
       </c>
     </row>
     <row r="68">
@@ -1121,7 +1166,7 @@
         <v>68</v>
       </c>
       <c r="B68" t="n">
-        <v>0.992195202103187</v>
+        <v>0.995695435864157</v>
       </c>
     </row>
     <row r="69">
@@ -1129,7 +1174,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="n">
-        <v>0.987471245481433</v>
+        <v>0.993121349772875</v>
       </c>
     </row>
     <row r="70">
@@ -1137,7 +1182,7 @@
         <v>70</v>
       </c>
       <c r="B70" t="n">
-        <v>0.988621426224121</v>
+        <v>0.993813540990699</v>
       </c>
     </row>
     <row r="71">
@@ -1145,7 +1190,7 @@
         <v>71</v>
       </c>
       <c r="B71" t="n">
-        <v>0.987553401248767</v>
+        <v>0.993034825870647</v>
       </c>
     </row>
     <row r="72">
@@ -1153,7 +1198,7 @@
         <v>72</v>
       </c>
       <c r="B72" t="n">
-        <v>0.989360828130134</v>
+        <v>0.994116374648497</v>
       </c>
     </row>
     <row r="73">
@@ -1161,7 +1206,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="n">
-        <v>0.987142622412093</v>
+        <v>0.992731992212849</v>
       </c>
     </row>
     <row r="74">
@@ -1169,7 +1214,7 @@
         <v>74</v>
       </c>
       <c r="B74" t="n">
-        <v>0.9857459743674</v>
+        <v>0.992299372701709</v>
       </c>
     </row>
     <row r="75">
@@ -1177,7 +1222,7 @@
         <v>75</v>
       </c>
       <c r="B75" t="n">
-        <v>0.987471245481433</v>
+        <v>0.993207873675103</v>
       </c>
     </row>
     <row r="76">
@@ -1185,7 +1230,7 @@
         <v>76</v>
       </c>
       <c r="B76" t="n">
-        <v>0.987882024318107</v>
+        <v>0.993207873675103</v>
       </c>
     </row>
     <row r="77">
@@ -1193,7 +1238,7 @@
         <v>77</v>
       </c>
       <c r="B77" t="n">
-        <v>0.988210647387446</v>
+        <v>0.993597231235129</v>
       </c>
     </row>
     <row r="78">
@@ -1201,7 +1246,127 @@
         <v>78</v>
       </c>
       <c r="B78" t="n">
-        <v>0.917269142293789</v>
+        <v>0.76707765520225</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79" t="n">
+        <v>0.952563270603504</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>80</v>
+      </c>
+      <c r="B80" t="n">
+        <v>0.762773091066407</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81" t="n">
+        <v>0.625567813108371</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>82</v>
+      </c>
+      <c r="B82" t="n">
+        <v>0.697252866104261</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>83</v>
+      </c>
+      <c r="B83" t="n">
+        <v>0.697252866104261</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>84</v>
+      </c>
+      <c r="B84" t="n">
+        <v>0.697252866104261</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>85</v>
+      </c>
+      <c r="B85" t="n">
+        <v>0.950703006705602</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>86</v>
+      </c>
+      <c r="B86" t="n">
+        <v>0.714233181916504</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>87</v>
+      </c>
+      <c r="B87" t="n">
+        <v>0.863962794722042</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>88</v>
+      </c>
+      <c r="B88" t="n">
+        <v>0.974432186891629</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>89</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0.698615617564352</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>90</v>
+      </c>
+      <c r="B90" t="n">
+        <v>0.697901795370971</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>91</v>
+      </c>
+      <c r="B91" t="n">
+        <v>0.90893359290504</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>92</v>
+      </c>
+      <c r="B92" t="n">
+        <v>0.70194678780013</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>93</v>
+      </c>
+      <c r="B93" t="n">
+        <v>0.871533636166991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>